<commit_message>
Uprade:    -Skip '%' in Config Header
</commit_message>
<xml_diff>
--- a/Smartsheet/Config.xlsx
+++ b/Smartsheet/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet_v0p5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C76A2A0-97E8-4F1D-855E-D646950FEEF1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3127F2DD-CD0A-46D0-B1EB-B25CA13DFF72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="164">
   <si>
     <t>No.</t>
   </si>
@@ -463,15 +463,6 @@
     <t>NRE_s027</t>
   </si>
   <si>
-    <t>NRE_A009</t>
-  </si>
-  <si>
-    <t>NRE_s020_SDLL</t>
-  </si>
-  <si>
-    <t>NRE_S023</t>
-  </si>
-  <si>
     <t>anhhoang@savarti.com</t>
   </si>
   <si>
@@ -518,6 +509,18 @@
   </si>
   <si>
     <t>2019-05-3</t>
+  </si>
+  <si>
+    <t>NRE_a009</t>
+  </si>
+  <si>
+    <t>NRE_s020_sdll</t>
+  </si>
+  <si>
+    <t>NRE_s023</t>
+  </si>
+  <si>
+    <t>NRE_ECC_cpl</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1318,14 +1321,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="37" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
@@ -1342,7 +1345,7 @@
         <v>102</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1721,7 +1724,7 @@
         <v>104</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2233,7 +2236,7 @@
         <v>103</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2918,7 +2921,7 @@
         <v>104</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2935,7 +2938,7 @@
         <v>104</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3086,8 +3089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0036914-8F78-4F8A-B32E-27D323C3EABC}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,7 +3108,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -3118,7 +3121,7 @@
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>136</v>
@@ -3158,7 +3161,7 @@
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>137</v>
@@ -3170,41 +3173,41 @@
         <v>137</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
@@ -3278,7 +3281,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>123</v>
@@ -3307,7 +3310,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>123</v>
@@ -3336,7 +3339,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>123</v>
@@ -3361,15 +3364,33 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
+      <c r="A12" s="30">
+        <v>5</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>

</xml_diff>

<commit_message>
fix notification when sheet Config is not exist in smartsheet
</commit_message>
<xml_diff>
--- a/Smartsheet/Config.xlsx
+++ b/Smartsheet/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3127F2DD-CD0A-46D0-B1EB-B25CA13DFF72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36326B76-4BFF-4C96-9E58-FA3F1DEC180A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="160">
   <si>
     <t>No.</t>
   </si>
@@ -460,9 +460,6 @@
     <t>Hoang Dinh Nhuan</t>
   </si>
   <si>
-    <t>NRE_s027</t>
-  </si>
-  <si>
     <t>anhhoang@savarti.com</t>
   </si>
   <si>
@@ -509,15 +506,6 @@
   </si>
   <si>
     <t>2019-05-3</t>
-  </si>
-  <si>
-    <t>NRE_a009</t>
-  </si>
-  <si>
-    <t>NRE_s020_sdll</t>
-  </si>
-  <si>
-    <t>NRE_s023</t>
   </si>
   <si>
     <t>NRE_ECC_cpl</t>
@@ -1321,14 +1309,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
@@ -1345,7 +1333,7 @@
         <v>102</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1724,7 +1712,7 @@
         <v>104</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2236,7 +2224,7 @@
         <v>103</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2921,7 +2909,7 @@
         <v>104</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2938,7 +2926,7 @@
         <v>104</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3090,7 +3078,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,7 +3096,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -3121,7 +3109,7 @@
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>136</v>
@@ -3161,7 +3149,7 @@
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>137</v>
@@ -3173,41 +3161,41 @@
         <v>137</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
@@ -3249,10 +3237,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>123</v>
@@ -3277,120 +3265,37 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
-        <v>2</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>130</v>
-      </c>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
-        <v>3</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>130</v>
-      </c>
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
-        <v>4</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
-        <v>5</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="I12" s="31" t="s">
-        <v>130</v>
-      </c>
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
@@ -3648,12 +3553,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B4E479002A54044887D55D48426EDAE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e67c679f2be2e66c3dc03d22eead815">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ab65288-7646-42de-b0ad-1a655932d5d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a9696e79b09e5e51dbcfe4378b974b2" ns2:_="">
     <xsd:import namespace="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
@@ -3797,6 +3696,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
   <ds:schemaRefs>
@@ -3806,22 +3711,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF46D3B7-820B-464E-96C4-8E1239941AAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3837,4 +3726,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add list holiday add Monthly timesheet and weekly timesheet
</commit_message>
<xml_diff>
--- a/Smartsheet/Config.xlsx
+++ b/Smartsheet/Config.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36326B76-4BFF-4C96-9E58-FA3F1DEC180A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5EF73-CEC1-47EE-81AC-E074D4940327}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="3" r:id="rId2"/>
+    <sheet name="Holiday" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="174">
   <si>
     <t>No.</t>
   </si>
@@ -478,37 +479,79 @@
     <t>Other Info</t>
   </si>
   <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>toannguyen@savarti.com, huutoanphophong@gmail.com, Toan Nguyen</t>
+  </si>
+  <si>
+    <t>nhuanhoang@savarti.com, Nhuan Hoang</t>
+  </si>
+  <si>
+    <t>F1:H29A1F1:I26F1:H34F1:H40A1F1:I26FF1:H99</t>
+  </si>
+  <si>
+    <t>-----------------------------Don't insert new colum. This row (1) and row  2 are default, don't touch-----------------------------------</t>
+  </si>
+  <si>
+    <t>--------------------------------------------------------------------------------------------Define headers name----------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>----------------------------------------------------------------Don't insert new colum. Only insert new row bellow row number 7-----------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Allocation %</t>
+  </si>
+  <si>
+    <t>Complete %</t>
+  </si>
+  <si>
+    <t>%Complete</t>
+  </si>
+  <si>
+    <t>NRE_A009</t>
+  </si>
+  <si>
+    <t>NRE_P910_revA</t>
+  </si>
+  <si>
+    <t>NRE_ECC_CPL</t>
+  </si>
+  <si>
+    <t>NRE_s005</t>
+  </si>
+  <si>
+    <t>NRE_s020_SDLL</t>
+  </si>
+  <si>
+    <t>NRE_S021</t>
+  </si>
+  <si>
+    <t>NRE_S023</t>
+  </si>
+  <si>
+    <t>NRE_S024</t>
+  </si>
+  <si>
+    <t>NRE_s027</t>
+  </si>
+  <si>
+    <t>NRE_P912_Ecoxip64M</t>
+  </si>
+  <si>
+    <t>NRE_A010</t>
+  </si>
+  <si>
     <t>2019-3-1</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>toannguyen@savarti.com, huutoanphophong@gmail.com, Toan Nguyen</t>
-  </si>
-  <si>
-    <t>nhuanhoang@savarti.com, Nhuan Hoang</t>
-  </si>
-  <si>
-    <t>F1:H29A1F1:I26F1:H34F1:H40A1F1:I26FF1:H99</t>
-  </si>
-  <si>
-    <t>-----------------------------Don't insert new colum. This row (1) and row  2 are default, don't touch-----------------------------------</t>
-  </si>
-  <si>
-    <t>--------------------------------------------------------------------------------------------Define headers name----------------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>----------------------------------------------------------------Don't insert new colum. Only insert new row bellow row number 7-----------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>2019-05-3</t>
-  </si>
-  <si>
-    <t>NRE_ECC_cpl</t>
+    <t>2019-06-15</t>
+  </si>
+  <si>
+    <t>Holiday</t>
   </si>
 </sst>
 </file>
@@ -519,7 +562,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,8 +650,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,6 +723,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,7 +899,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -925,6 +988,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1292,31 +1380,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="16" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="16"/>
     <col min="4" max="4" width="9.140625" style="27"/>
     <col min="5" max="5" width="102.5703125" style="20" customWidth="1"/>
-    <col min="6" max="10" width="9.140625" style="37"/>
+    <col min="6" max="10" width="9.140625" style="46"/>
     <col min="11" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
-        <v>154</v>
+      <c r="A1" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
@@ -2909,7 +2997,7 @@
         <v>104</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -2926,7 +3014,7 @@
         <v>104</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3075,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0036914-8F78-4F8A-B32E-27D323C3EABC}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="A8:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3095,41 +3183,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="A1" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="49" t="s">
         <v>132</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="9" t="s">
         <v>135</v>
       </c>
@@ -3142,8 +3230,8 @@
       <c r="E3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
@@ -3158,16 +3246,16 @@
         <v>140</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -3180,31 +3268,31 @@
         <v>140</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="A6" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -3237,10 +3325,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
-        <v>5</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>159</v>
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>123</v>
@@ -3258,121 +3346,330 @@
         <v>128</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="I8" s="31" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
+      <c r="A9" s="30">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
+      <c r="A10" s="30">
+        <v>3</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
+      <c r="A11" s="30">
+        <v>4</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
+      <c r="A14" s="30">
+        <v>8</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="A16" s="30">
+        <v>10</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="A17" s="30">
+        <v>11</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
+      <c r="A18" s="30">
+        <v>12</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
+      <c r="A19" s="30">
+        <v>13</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
@@ -3527,6 +3824,28 @@
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
       <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3543,6 +3862,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F991957B-BA63-4B65-BE29-24E281DEF62D}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42">
+        <v>43500</v>
+      </c>
+      <c r="C2" s="38"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42">
+        <v>43501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>3</v>
+      </c>
+      <c r="B4" s="42">
+        <v>43502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
+        <v>4</v>
+      </c>
+      <c r="B5" s="42">
+        <v>43503</v>
+      </c>
+      <c r="C5" s="38"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>5</v>
+      </c>
+      <c r="B6" s="41">
+        <v>43504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
+        <v>6</v>
+      </c>
+      <c r="B7" s="41">
+        <v>43570</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>7</v>
+      </c>
+      <c r="B8" s="41">
+        <v>43585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
+        <v>8</v>
+      </c>
+      <c r="B9" s="41">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
+        <v>9</v>
+      </c>
+      <c r="B10" s="41">
+        <v>43710</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3553,6 +3984,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B4E479002A54044887D55D48426EDAE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e67c679f2be2e66c3dc03d22eead815">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ab65288-7646-42de-b0ad-1a655932d5d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a9696e79b09e5e51dbcfe4378b974b2" ns2:_="">
     <xsd:import namespace="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
@@ -3696,12 +4133,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
   <ds:schemaRefs>
@@ -3711,6 +4142,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF46D3B7-820B-464E-96C4-8E1239941AAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3726,20 +4173,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add 2 new sheet (new  format)
</commit_message>
<xml_diff>
--- a/Smartsheet/Config.xlsx
+++ b/Smartsheet/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5EF73-CEC1-47EE-81AC-E074D4940327}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F6797E-C09E-404E-9CDE-2F0B2A664657}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="182">
   <si>
     <t>No.</t>
   </si>
   <si>
-    <t xml:space="preserve">Full name </t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>Luong Nguyen</t>
   </si>
   <si>
-    <t>Circuit</t>
-  </si>
-  <si>
     <t>Tan Nguyen</t>
   </si>
   <si>
@@ -71,9 +62,6 @@
     <t>Loc Ho</t>
   </si>
   <si>
-    <t>Layout</t>
-  </si>
-  <si>
     <t>Truong Nguyen</t>
   </si>
   <si>
@@ -212,9 +200,6 @@
     <t>Linh Tong</t>
   </si>
   <si>
-    <t>Hang Hoang</t>
-  </si>
-  <si>
     <t>Quoc Ha</t>
   </si>
   <si>
@@ -338,9 +323,6 @@
     <t>Nguyen Trong Tuan</t>
   </si>
   <si>
-    <t>Seniority level</t>
-  </si>
-  <si>
     <t>Sr</t>
   </si>
   <si>
@@ -395,9 +377,6 @@
     <t>Thuan Trang</t>
   </si>
   <si>
-    <t>Vo Huynh Thai Duong</t>
-  </si>
-  <si>
     <t>Sheet name</t>
   </si>
   <si>
@@ -431,9 +410,6 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>% Complete</t>
-  </si>
-  <si>
     <t>Filter by month</t>
   </si>
   <si>
@@ -500,58 +476,106 @@
     <t>----------------------------------------------------------------Don't insert new colum. Only insert new row bellow row number 7-----------------------------------------------------------------</t>
   </si>
   <si>
+    <t>Allocation %</t>
+  </si>
+  <si>
+    <t>Complete %</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>NRE_s028</t>
+  </si>
+  <si>
+    <t>Duong Vo</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Design Manager</t>
+  </si>
+  <si>
+    <t>Sr. Engineer</t>
+  </si>
+  <si>
+    <t>CKT</t>
+  </si>
+  <si>
+    <t>Jr. Engineer</t>
+  </si>
+  <si>
+    <t>LAY</t>
+  </si>
+  <si>
+    <t>Hang Nguyen</t>
+  </si>
+  <si>
+    <t>Filter by user (new format)</t>
+  </si>
+  <si>
+    <t>NRE_S030</t>
+  </si>
+  <si>
+    <t>NRE_XFLASH7</t>
+  </si>
+  <si>
+    <t>NRE_s020_SDLL</t>
+  </si>
+  <si>
     <t>Complete</t>
   </si>
   <si>
-    <t>Allocation %</t>
-  </si>
-  <si>
-    <t>Complete %</t>
-  </si>
-  <si>
-    <t>%Complete</t>
+    <t>NRE_s027</t>
+  </si>
+  <si>
+    <t>NRE_S023</t>
   </si>
   <si>
     <t>NRE_A009</t>
   </si>
   <si>
+    <t>NRE_A010</t>
+  </si>
+  <si>
+    <t>2019-1-1</t>
+  </si>
+  <si>
+    <t>NRE_s002</t>
+  </si>
+  <si>
     <t>NRE_P910_revA</t>
   </si>
   <si>
+    <t>NRE_P912_Ecoxip64M</t>
+  </si>
+  <si>
+    <t>NRE_s005</t>
+  </si>
+  <si>
     <t>NRE_ECC_CPL</t>
   </si>
   <si>
-    <t>NRE_s005</t>
-  </si>
-  <si>
-    <t>NRE_s020_SDLL</t>
-  </si>
-  <si>
-    <t>NRE_S021</t>
-  </si>
-  <si>
-    <t>NRE_S023</t>
-  </si>
-  <si>
-    <t>NRE_S024</t>
-  </si>
-  <si>
-    <t>NRE_s027</t>
-  </si>
-  <si>
-    <t>NRE_P912_Ecoxip64M</t>
-  </si>
-  <si>
-    <t>NRE_A010</t>
-  </si>
-  <si>
-    <t>2019-3-1</t>
-  </si>
-  <si>
-    <t>2019-06-15</t>
-  </si>
-  <si>
-    <t>Holiday</t>
+    <t>RnD_N16_2PTCAM</t>
+  </si>
+  <si>
+    <t>RnD_P2P_BIST</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>2019-12-30</t>
   </si>
 </sst>
 </file>
@@ -899,7 +923,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1016,10 +1040,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1060,6 +1084,13 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="11" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1380,16 +1411,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="16"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="3" max="3" width="9.140625" style="27"/>
+    <col min="4" max="4" width="23.85546875" style="16" customWidth="1"/>
     <col min="5" max="5" width="102.5703125" style="20" customWidth="1"/>
     <col min="6" max="10" width="9.140625" style="46"/>
     <col min="11" max="16384" width="9.140625" style="16"/>
@@ -1397,31 +1428,31 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1429,13 +1460,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>103</v>
+        <v>152</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -1444,16 +1475,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>103</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1461,13 +1492,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>103</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E5" s="7"/>
     </row>
@@ -1476,13 +1507,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>103</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -1491,13 +1522,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>104</v>
+        <v>54</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -1506,13 +1537,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>104</v>
+        <v>91</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -1521,13 +1552,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>103</v>
+        <v>34</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -1536,28 +1567,30 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>103</v>
+        <v>38</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E11" s="7"/>
     </row>
@@ -1566,13 +1599,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>103</v>
+        <v>89</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -1581,13 +1614,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>104</v>
+        <v>55</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -1596,13 +1629,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>104</v>
+        <v>162</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E14" s="7"/>
     </row>
@@ -1611,13 +1644,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E15" s="7"/>
     </row>
@@ -1626,13 +1659,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -1641,13 +1674,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>103</v>
+        <v>35</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E17" s="7"/>
     </row>
@@ -1656,13 +1689,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>103</v>
+        <v>50</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E18" s="7"/>
     </row>
@@ -1671,13 +1704,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>103</v>
+      <c r="C19" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E19" s="7"/>
     </row>
@@ -1686,13 +1719,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>104</v>
+        <v>71</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -1701,13 +1734,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -1716,13 +1749,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="25" t="s">
         <v>104</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -1731,13 +1764,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>104</v>
+        <v>51</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E23" s="7"/>
     </row>
@@ -1746,13 +1779,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E24" s="7"/>
     </row>
@@ -1761,13 +1794,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>103</v>
+        <v>40</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E25" s="7"/>
     </row>
@@ -1776,13 +1809,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>103</v>
+        <v>37</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -1791,16 +1824,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>104</v>
+        <v>90</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1808,13 +1841,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>104</v>
+        <v>65</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E28" s="7"/>
     </row>
@@ -1823,13 +1856,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>104</v>
+        <v>66</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E29" s="7"/>
     </row>
@@ -1838,13 +1871,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>103</v>
+        <v>4</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E30" s="7"/>
     </row>
@@ -1853,13 +1886,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E31" s="7"/>
     </row>
@@ -1868,13 +1901,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>103</v>
+        <v>36</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E32" s="7"/>
     </row>
@@ -1883,13 +1916,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E33" s="7"/>
     </row>
@@ -1898,13 +1931,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E34" s="7"/>
     </row>
@@ -1913,13 +1946,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>103</v>
+        <v>6</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E35" s="7"/>
     </row>
@@ -1928,13 +1961,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>103</v>
+        <v>21</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E36" s="7"/>
     </row>
@@ -1943,13 +1976,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E37" s="7"/>
     </row>
@@ -1958,13 +1991,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E38" s="7"/>
     </row>
@@ -1973,13 +2006,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>103</v>
+        <v>27</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E39" s="7"/>
     </row>
@@ -1988,13 +2021,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>104</v>
+        <v>47</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E40" s="7"/>
     </row>
@@ -2003,13 +2036,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>103</v>
+        <v>11</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E41" s="7"/>
     </row>
@@ -2018,13 +2051,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>104</v>
+        <v>75</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E42" s="7"/>
     </row>
@@ -2033,13 +2066,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>103</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="E43" s="7"/>
     </row>
@@ -2048,13 +2081,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="E44" s="7"/>
     </row>
@@ -2063,13 +2096,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>103</v>
+        <v>17</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E45" s="7"/>
     </row>
@@ -2078,13 +2111,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>103</v>
+        <v>15</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E46" s="7"/>
     </row>
@@ -2093,13 +2126,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>104</v>
+        <v>80</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E47" s="7"/>
     </row>
@@ -2108,13 +2141,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>104</v>
+        <v>72</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E48" s="7"/>
     </row>
@@ -2123,13 +2156,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>104</v>
+        <v>79</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E49" s="7"/>
     </row>
@@ -2138,13 +2171,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E50" s="7"/>
     </row>
@@ -2153,13 +2186,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>104</v>
+        <v>53</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E51" s="7"/>
     </row>
@@ -2168,13 +2201,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>103</v>
+        <v>23</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E52" s="7"/>
     </row>
@@ -2183,13 +2216,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E53" s="7"/>
     </row>
@@ -2198,13 +2231,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E54" s="7"/>
     </row>
@@ -2213,13 +2246,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E55" s="7"/>
     </row>
@@ -2228,13 +2261,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>104</v>
+        <v>64</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E56" s="7"/>
     </row>
@@ -2243,13 +2276,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>104</v>
+        <v>112</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E57" s="7"/>
     </row>
@@ -2258,13 +2291,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>103</v>
+        <v>20</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E58" s="7"/>
     </row>
@@ -2273,13 +2306,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>103</v>
+        <v>13</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E59" s="7"/>
     </row>
@@ -2288,13 +2321,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>103</v>
+        <v>14</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E60" s="7"/>
     </row>
@@ -2303,16 +2336,16 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>103</v>
+        <v>48</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2320,13 +2353,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>104</v>
+        <v>73</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E62" s="7"/>
     </row>
@@ -2335,13 +2368,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E63" s="7"/>
     </row>
@@ -2350,13 +2383,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E64" s="7"/>
     </row>
@@ -2365,13 +2398,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>104</v>
+        <v>45</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E65" s="7"/>
     </row>
@@ -2380,13 +2413,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>103</v>
+        <v>81</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E66" s="7"/>
     </row>
@@ -2395,13 +2428,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E67" s="7"/>
     </row>
@@ -2410,13 +2443,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>103</v>
+        <v>9</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="E68" s="7"/>
     </row>
@@ -2425,13 +2458,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>103</v>
+        <v>12</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E69" s="7"/>
     </row>
@@ -2440,13 +2473,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>104</v>
+        <v>58</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E70" s="7"/>
     </row>
@@ -2455,13 +2488,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="25" t="s">
-        <v>104</v>
+        <v>59</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E71" s="7"/>
     </row>
@@ -2470,13 +2503,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="25" t="s">
-        <v>104</v>
+        <v>60</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E72" s="7"/>
     </row>
@@ -2485,13 +2518,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="25" t="s">
-        <v>104</v>
+        <v>61</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E73" s="7"/>
     </row>
@@ -2500,13 +2533,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="25" t="s">
-        <v>104</v>
+        <v>62</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E74" s="7"/>
     </row>
@@ -2515,13 +2548,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="25" t="s">
-        <v>104</v>
+        <v>44</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E75" s="7"/>
     </row>
@@ -2530,13 +2563,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="25" t="s">
-        <v>103</v>
+        <v>5</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E76" s="7"/>
     </row>
@@ -2545,13 +2578,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" s="25" t="s">
-        <v>103</v>
+        <v>6</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E77" s="7"/>
     </row>
@@ -2560,13 +2593,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D78" s="25" t="s">
-        <v>103</v>
+      <c r="C78" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E78" s="7"/>
     </row>
@@ -2575,13 +2608,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" s="25" t="s">
-        <v>103</v>
+        <v>18</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E79" s="7"/>
     </row>
@@ -2590,13 +2623,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="25" t="s">
-        <v>104</v>
+        <v>22</v>
+      </c>
+      <c r="C80" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E80" s="7"/>
     </row>
@@ -2605,13 +2638,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D81" s="25" t="s">
-        <v>103</v>
+        <v>24</v>
+      </c>
+      <c r="C81" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E81" s="7"/>
     </row>
@@ -2620,13 +2653,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D82" s="25" t="s">
-        <v>104</v>
+        <v>32</v>
+      </c>
+      <c r="C82" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E82" s="7"/>
     </row>
@@ -2635,13 +2668,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="25" t="s">
-        <v>104</v>
+        <v>33</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E83" s="7"/>
     </row>
@@ -2650,13 +2683,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="25" t="s">
-        <v>104</v>
+        <v>42</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E84" s="7"/>
     </row>
@@ -2665,13 +2698,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="25" t="s">
-        <v>104</v>
+        <v>43</v>
+      </c>
+      <c r="C85" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E85" s="7"/>
     </row>
@@ -2680,13 +2713,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" s="25" t="s">
-        <v>104</v>
+        <v>52</v>
+      </c>
+      <c r="C86" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E86" s="7"/>
     </row>
@@ -2695,13 +2728,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D87" s="25" t="s">
-        <v>104</v>
+        <v>56</v>
+      </c>
+      <c r="C87" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="E87" s="7"/>
     </row>
@@ -2710,13 +2743,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" s="25" t="s">
-        <v>103</v>
+        <v>63</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E88" s="7"/>
     </row>
@@ -2725,13 +2758,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D89" s="25" t="s">
-        <v>104</v>
+        <v>71</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E89" s="7"/>
     </row>
@@ -2740,13 +2773,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="25" t="s">
-        <v>104</v>
+        <v>74</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E90" s="7"/>
     </row>
@@ -2755,13 +2788,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" s="25" t="s">
-        <v>104</v>
+        <v>76</v>
+      </c>
+      <c r="C91" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E91" s="7"/>
     </row>
@@ -2770,13 +2803,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D92" s="25" t="s">
-        <v>103</v>
+        <v>78</v>
+      </c>
+      <c r="C92" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E92" s="7"/>
     </row>
@@ -2785,13 +2818,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="25" t="s">
-        <v>103</v>
+        <v>82</v>
+      </c>
+      <c r="C93" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E93" s="7"/>
     </row>
@@ -2800,12 +2833,12 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D94" s="25"/>
+        <v>67</v>
+      </c>
+      <c r="C94" s="25"/>
+      <c r="D94" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2813,12 +2846,12 @@
         <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D95" s="25"/>
+        <v>69</v>
+      </c>
+      <c r="C95" s="25"/>
+      <c r="D95" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2826,12 +2859,12 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D96" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="C96" s="25"/>
+      <c r="D96" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2839,12 +2872,12 @@
         <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D97" s="25"/>
+        <v>25</v>
+      </c>
+      <c r="C97" s="25"/>
+      <c r="D97" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2852,12 +2885,12 @@
         <v>96</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D98" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="C98" s="25"/>
+      <c r="D98" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -2865,12 +2898,12 @@
         <v>97</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D99" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="C99" s="25"/>
+      <c r="D99" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -2878,12 +2911,12 @@
         <v>98</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D100" s="25"/>
+        <v>77</v>
+      </c>
+      <c r="C100" s="25"/>
+      <c r="D100" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2891,12 +2924,12 @@
         <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D101" s="25"/>
+        <v>84</v>
+      </c>
+      <c r="C101" s="25"/>
+      <c r="D101" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E101" s="7"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -2904,12 +2937,12 @@
         <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D102" s="25"/>
+        <v>85</v>
+      </c>
+      <c r="C102" s="25"/>
+      <c r="D102" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -2917,12 +2950,12 @@
         <v>101</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D103" s="25"/>
+        <v>86</v>
+      </c>
+      <c r="C103" s="25"/>
+      <c r="D103" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E103" s="7"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2930,12 +2963,12 @@
         <v>102</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D104" s="25"/>
+        <v>88</v>
+      </c>
+      <c r="C104" s="25"/>
+      <c r="D104" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="E104" s="7"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -2943,13 +2976,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" s="25" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="C105" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="E105" s="7"/>
     </row>
@@ -2958,13 +2991,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D106" s="25" t="s">
-        <v>103</v>
+        <v>93</v>
+      </c>
+      <c r="C106" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E106" s="7"/>
     </row>
@@ -2973,13 +3006,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D107" s="25" t="s">
-        <v>104</v>
+        <v>114</v>
+      </c>
+      <c r="C107" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E107" s="7"/>
     </row>
@@ -2988,16 +3021,16 @@
         <v>106</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -3005,156 +3038,164 @@
         <v>107</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="5"/>
       <c r="E110" s="7"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="5"/>
       <c r="E111" s="7"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="5"/>
       <c r="E112" s="7"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="5"/>
       <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="18"/>
       <c r="B114" s="18"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="18"/>
       <c r="E114" s="19"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="18"/>
       <c r="B115" s="18"/>
-      <c r="C115" s="18"/>
-      <c r="D115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="18"/>
       <c r="E115" s="19"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="18"/>
       <c r="B116" s="18"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="26"/>
+      <c r="C116" s="26"/>
+      <c r="D116" s="18"/>
       <c r="E116" s="19"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="18"/>
       <c r="B117" s="18"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="26"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="18"/>
       <c r="E117" s="19"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="18"/>
       <c r="B118" s="18"/>
-      <c r="C118" s="18"/>
-      <c r="D118" s="26"/>
+      <c r="C118" s="26"/>
+      <c r="D118" s="18"/>
       <c r="E118" s="19"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="18"/>
       <c r="B119" s="18"/>
-      <c r="C119" s="18"/>
-      <c r="D119" s="26"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="18"/>
       <c r="E119" s="19"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="18"/>
       <c r="B120" s="18"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="26"/>
+      <c r="C120" s="26"/>
+      <c r="D120" s="18"/>
       <c r="E120" s="19"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="18"/>
       <c r="B121" s="18"/>
-      <c r="C121" s="18"/>
-      <c r="D121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="18"/>
       <c r="E121" s="19"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="18"/>
       <c r="B122" s="18"/>
-      <c r="C122" s="18"/>
-      <c r="D122" s="26"/>
+      <c r="C122" s="26"/>
+      <c r="D122" s="18"/>
       <c r="E122" s="19"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="18"/>
       <c r="B123" s="18"/>
-      <c r="C123" s="18"/>
-      <c r="D123" s="26"/>
+      <c r="C123" s="26"/>
+      <c r="D123" s="18"/>
       <c r="E123" s="19"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="18"/>
       <c r="B124" s="18"/>
-      <c r="C124" s="18"/>
-      <c r="D124" s="26"/>
+      <c r="C124" s="26"/>
+      <c r="D124" s="18"/>
       <c r="E124" s="19"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="18"/>
       <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="26"/>
+      <c r="C125" s="26"/>
+      <c r="D125" s="18"/>
       <c r="E125" s="19"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D96">
     <sortCondition ref="A2"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="1">
     <mergeCell ref="F1:J1048576"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106:C107 C5:C102" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D82 D20:D24 D17:D18 D65 D46:D57 D43:D44 D94:D102 D77 D79 D92 D84 D86:D87 D89" xr:uid="{474471D3-EE3D-4F77-B72D-F428998DD97F}">
       <formula1>"RTL, UVM, PD, Circuit, Layout, CAD, Contractor, Trainer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C68" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"RTL, UVM, PD, Circuit, Layout, CAD, SI, PCB,Contractor, Trainer"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103:C104 C97 C106:C107 C57:C75" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D103:D104 D97 D65 D57" xr:uid="{9CAD9E53-8AC1-4028-9877-0DE0FCFFD764}">
       <formula1>"RTL, UVM, PD, Circuit, Layout, CAD, Labtest, Contractor, Trainer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C97 C106:C107 C53:C75" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D97 D65 D53:D57" xr:uid="{FCB35022-340B-46BE-B967-A0A27E509C62}">
       <formula1>"RTL, UVM, PD, Circuit, Layout, CAD, QA, Contractor, Trainer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D59:D64 D66:D67 D76 D78 D80 D83 D85 D88 D90:D91 D93 D105" xr:uid="{73D5C66C-5534-452F-8E88-605933B1A73D}">
+      <formula1>"RTL, UVM, PD, CKT, LAY, CAD, QA, Contractor, Trainer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D59:D64 D66:D67 D76 D78 D80 D83 D85 D88 D90:D91 D93 D105" xr:uid="{365ADDD8-930C-4546-A51B-A8EE12E82ECD}">
+      <formula1>"RTL, UVM, PD, CKT, LAY, CAD, Labtest, Contractor, Trainer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D16 D25:D29 D31:D38 D40:D42 D59:D64 D66:D67 D78 D80:D81 D83 D85 D88 D90:D91 D93 D69:D76 D105:D107" xr:uid="{5494C7BB-AE7F-4FC6-A8A4-A667A8F68598}">
+      <formula1>"RTL, UVM, PD, CKT, LAY, CAD, Contractor, Trainer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D10" xr:uid="{7D74E5F7-B212-4D78-A3E6-B6BCF24FB13D}">
+      <formula1>"RTL, UVM, PD, CKT, LAY, CAD, DFT, Contractor, Trainer"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E108" r:id="rId1" display="toannnguyen@savarti.com" xr:uid="{4A172A09-D64E-44F6-A734-8E47A192AC58}"/>
-    <hyperlink ref="E109" r:id="rId2" xr:uid="{5729BBF5-43E1-4C6D-996D-ED3E20A1AF4B}"/>
-    <hyperlink ref="E27" r:id="rId3" xr:uid="{0ABB8BC5-A5EE-40E7-822E-9A38DFA84244}"/>
+    <hyperlink ref="E108" r:id="rId1" display="toannnguyen@savarti.com" xr:uid="{A84174A0-66FF-4B85-B024-42D34CDE4001}"/>
+    <hyperlink ref="E109" r:id="rId2" xr:uid="{B96A7A69-0277-41E4-966D-0EBF09CA7D1E}"/>
+    <hyperlink ref="E27" r:id="rId3" xr:uid="{82434C86-38F9-42D2-AF70-AD063A495D93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -3163,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0036914-8F78-4F8A-B32E-27D323C3EABC}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="A8:I19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,8 +3216,8 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -3184,7 +3225,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -3197,93 +3238,103 @@
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C2" s="54"/>
       <c r="D2" s="55" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E2" s="56"/>
-      <c r="F2" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="F2" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="56"/>
+      <c r="H2" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="57"/>
       <c r="B3" s="9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="G4" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="34" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="28" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
@@ -3299,86 +3350,86 @@
         <v>0</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>129</v>
-      </c>
       <c r="I7" s="13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>161</v>
+      <c r="B8" s="31" t="s">
+        <v>151</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D8" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G8" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>169</v>
+      <c r="B9" s="31" t="s">
+        <v>164</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D9" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G9" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,28 +3437,28 @@
         <v>3</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D10" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G10" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3415,294 +3466,348 @@
         <v>4</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C11" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11" s="31" t="s">
         <v>123</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>162</v>
+      <c r="B12" s="31" t="s">
+        <v>168</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D12" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G12" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D13" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G13" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D14" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>132</v>
-      </c>
       <c r="G14" s="31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
+        <v>8</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="58">
         <v>9</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="31" t="s">
+      <c r="B16" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="G16" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="58">
         <v>10</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="31" t="s">
+      <c r="B17" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="G17" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
         <v>11</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="31" t="s">
+      <c r="B18" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="I17" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="G18" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
         <v>12</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="31" t="s">
+      <c r="B19" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="I18" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="G19" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="58">
         <v>13</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="31" t="s">
+      <c r="B20" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="I19" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
+      <c r="G20" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="A21" s="58">
+        <v>14</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+      <c r="A22" s="58">
+        <v>15</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
@@ -3737,125 +3842,16 @@
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3866,7 +3862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F991957B-BA63-4B65-BE29-24E281DEF62D}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -3882,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3975,23 +3971,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B4E479002A54044887D55D48426EDAE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e67c679f2be2e66c3dc03d22eead815">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ab65288-7646-42de-b0ad-1a655932d5d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a9696e79b09e5e51dbcfe4378b974b2" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B4E479002A54044887D55D48426EDAE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a77c242a546c918351b2614e40c42a32">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ab65288-7646-42de-b0ad-1a655932d5d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2def084828ae6b9ab72ab374d395891" ns2:_="">
     <xsd:import namespace="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -4133,32 +4114,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF46D3B7-820B-464E-96C4-8E1239941AAA}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6913C62B-27C1-446F-9D3F-0B15D19E1177}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4173,4 +4145,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add package into src_3rd
</commit_message>
<xml_diff>
--- a/Smartsheet/Config.xlsx
+++ b/Smartsheet/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toannguyen\SVI_Smartsheet\Smartsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0902F61A-26A5-4BE4-84F2-AFD458B3E85A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F0D380-8A75-48B3-AA54-D4C63E873D18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>No.</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>-------------------------------------------------------------------------------------------List sheet----------------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>ex1, ex2</t>
   </si>
   <si>
     <t>Vu Huynhsad</t>
@@ -1124,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1264,10 +1261,10 @@
         <v>105</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>31</v>
@@ -1279,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>65</v>
@@ -1309,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0036914-8F78-4F8A-B32E-27D323C3EABC}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1427,9 +1424,7 @@
         <v>62</v>
       </c>
       <c r="J4" s="41"/>
-      <c r="K4" s="42" t="s">
-        <v>70</v>
-      </c>
+      <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -2013,9 +2008,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2163,26 +2161,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2206,9 +2193,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6DAC1E-ABE8-4504-A431-5FC9F5EE3DAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F2D34C-3841-4818-B80C-425266708FF0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ab65288-7646-42de-b0ad-1a655932d5d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>